<commit_message>
Commit before adding the right DLL's
</commit_message>
<xml_diff>
--- a/QuestionsWebApplication/Daily updates.xlsx
+++ b/QuestionsWebApplication/Daily updates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -129,7 +129,13 @@
     <t>Task: Working on implementing the questions builder web app further</t>
   </si>
   <si>
-    <t>s</t>
+    <t>7.5 hours</t>
+  </si>
+  <si>
+    <t>Task: Working on implementing signalR and sorting the data</t>
+  </si>
+  <si>
+    <t>Self learning: Learned more about C# interfaces</t>
   </si>
 </sst>
 </file>
@@ -496,7 +502,7 @@
   <dimension ref="A1:C120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,14 +776,26 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3">
+        <v>44461</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="A26" s="3">
+        <v>44461</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>

</xml_diff>